<commit_message>
Fixed colored syndicate flairs
</commit_message>
<xml_diff>
--- a/Flair JS & CSS.xlsx
+++ b/Flair JS & CSS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="110" windowWidth="19140" windowHeight="7330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="110" windowWidth="19140" windowHeight="7330"/>
   </bookViews>
   <sheets>
     <sheet name="flair.js" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2242" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2292" uniqueCount="344">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -1421,8 +1421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H200"/>
   <sheetViews>
-    <sheetView topLeftCell="C182" workbookViewId="0">
-      <selection activeCell="C199" sqref="C199"/>
+    <sheetView tabSelected="1" topLeftCell="C131" workbookViewId="0">
+      <selection activeCell="H198" sqref="H133:H198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -4301,6 +4301,9 @@
       <c r="C151" s="1" t="s">
         <v>176</v>
       </c>
+      <c r="D151" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E151" s="1" t="s">
         <v>292</v>
       </c>
@@ -4309,7 +4312,7 @@
       </c>
       <c r="H151" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"150 sigilsflair syndicate-cephalon-suda-level-7-sigil-yellowMultivariate (Cephalon Suda) sigil (yellow)",</v>
+        <v>"150 sigilsflair syndicate-cephalon-suda-level-7-sigil-yellow": "Multivariate (Cephalon Suda) sigil (yellow)",</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.35">
@@ -4322,6 +4325,9 @@
       <c r="C152" s="1" t="s">
         <v>177</v>
       </c>
+      <c r="D152" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E152" s="1" t="s">
         <v>293</v>
       </c>
@@ -4330,7 +4336,7 @@
       </c>
       <c r="H152" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"151 sigilsflair syndicate-cephalon-suda-level-8-sigil-yellowLabryinth (Cephalon Suda) sigil (yellow)",</v>
+        <v>"151 sigilsflair syndicate-cephalon-suda-level-8-sigil-yellow": "Labryinth (Cephalon Suda) sigil (yellow)",</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.35">
@@ -4343,6 +4349,9 @@
       <c r="C153" s="1" t="s">
         <v>178</v>
       </c>
+      <c r="D153" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E153" s="1" t="s">
         <v>294</v>
       </c>
@@ -4351,7 +4360,7 @@
       </c>
       <c r="H153" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"152 sigilsflair syndicate-cephalon-suda-level-9-sigil-yellowHexan (Cephalon Suda) sigil (yellow)",</v>
+        <v>"152 sigilsflair syndicate-cephalon-suda-level-9-sigil-yellow": "Hexan (Cephalon Suda) sigil (yellow)",</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.35">
@@ -4364,6 +4373,9 @@
       <c r="C154" s="1" t="s">
         <v>179</v>
       </c>
+      <c r="D154" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E154" s="1" t="s">
         <v>295</v>
       </c>
@@ -4372,7 +4384,7 @@
       </c>
       <c r="H154" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"153 sigilsflair syndicate-cephalon-suda-level-10-sigil-yellowOracle (Cephalon Suda) sigil (yellow)",</v>
+        <v>"153 sigilsflair syndicate-cephalon-suda-level-10-sigil-yellow": "Oracle (Cephalon Suda) sigil (yellow)",</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.35">
@@ -4385,6 +4397,9 @@
       <c r="C155" s="1" t="s">
         <v>180</v>
       </c>
+      <c r="D155" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E155" s="1" t="s">
         <v>296</v>
       </c>
@@ -4393,7 +4408,7 @@
       </c>
       <c r="H155" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"154 sigilsflair syndicate-new-loka-sigil-greenNew Loka sigil (green)",</v>
+        <v>"154 sigilsflair syndicate-new-loka-sigil-green": "New Loka sigil (green)",</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.35">
@@ -4406,6 +4421,9 @@
       <c r="C156" s="1" t="s">
         <v>181</v>
       </c>
+      <c r="D156" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E156" s="1" t="s">
         <v>297</v>
       </c>
@@ -4414,7 +4432,7 @@
       </c>
       <c r="H156" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"155 sigilsflair syndicate-new-loka-level-1-sigil-greenSacrifice (New Loka) sigil (green)",</v>
+        <v>"155 sigilsflair syndicate-new-loka-level-1-sigil-green": "Sacrifice (New Loka) sigil (green)",</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.35">
@@ -4427,6 +4445,9 @@
       <c r="C157" s="1" t="s">
         <v>182</v>
       </c>
+      <c r="D157" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E157" s="1" t="s">
         <v>298</v>
       </c>
@@ -4435,7 +4456,7 @@
       </c>
       <c r="H157" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"156 sigilsflair syndicate-new-loka-level-2-sigil-greenSeed (New Loka) sigil (green)",</v>
+        <v>"156 sigilsflair syndicate-new-loka-level-2-sigil-green": "Seed (New Loka) sigil (green)",</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.35">
@@ -4448,6 +4469,9 @@
       <c r="C158" s="1" t="s">
         <v>183</v>
       </c>
+      <c r="D158" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E158" s="1" t="s">
         <v>299</v>
       </c>
@@ -4456,7 +4480,7 @@
       </c>
       <c r="H158" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"157 sigilsflair syndicate-new-loka-level-3-sigil-greenRebirth (New Loka) sigil (green)",</v>
+        <v>"157 sigilsflair syndicate-new-loka-level-3-sigil-green": "Rebirth (New Loka) sigil (green)",</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.35">
@@ -4469,6 +4493,9 @@
       <c r="C159" s="1" t="s">
         <v>184</v>
       </c>
+      <c r="D159" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E159" s="1" t="s">
         <v>300</v>
       </c>
@@ -4477,7 +4504,7 @@
       </c>
       <c r="H159" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"158 sigilsflair syndicate-new-loka-level-4-sigil-greenGrowth (New Loka) sigil (green)",</v>
+        <v>"158 sigilsflair syndicate-new-loka-level-4-sigil-green": "Growth (New Loka) sigil (green)",</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.35">
@@ -4490,6 +4517,9 @@
       <c r="C160" s="1" t="s">
         <v>185</v>
       </c>
+      <c r="D160" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E160" s="1" t="s">
         <v>301</v>
       </c>
@@ -4498,7 +4528,7 @@
       </c>
       <c r="H160" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"159 sigilsflair syndicate-new-loka-level-5-sigil-greenClarity (New Loka) sigil (green)",</v>
+        <v>"159 sigilsflair syndicate-new-loka-level-5-sigil-green": "Clarity (New Loka) sigil (green)",</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.35">
@@ -4511,6 +4541,9 @@
       <c r="C161" s="1" t="s">
         <v>186</v>
       </c>
+      <c r="D161" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E161" s="1" t="s">
         <v>302</v>
       </c>
@@ -4519,7 +4552,7 @@
       </c>
       <c r="H161" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"160 sigilsflair syndicate-new-loka-level-6-sigil-greenBloom (New Loka) sigil (green)",</v>
+        <v>"160 sigilsflair syndicate-new-loka-level-6-sigil-green": "Bloom (New Loka) sigil (green)",</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.35">
@@ -4532,6 +4565,9 @@
       <c r="C162" s="1" t="s">
         <v>187</v>
       </c>
+      <c r="D162" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E162" s="1" t="s">
         <v>303</v>
       </c>
@@ -4540,7 +4576,7 @@
       </c>
       <c r="H162" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"161 sigilsflair syndicate-new-loka-level-7-sigil-greenPurity (New Loka) sigil (green)",</v>
+        <v>"161 sigilsflair syndicate-new-loka-level-7-sigil-green": "Purity (New Loka) sigil (green)",</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.35">
@@ -4553,6 +4589,9 @@
       <c r="C163" s="1" t="s">
         <v>188</v>
       </c>
+      <c r="D163" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E163" s="1" t="s">
         <v>304</v>
       </c>
@@ -4561,7 +4600,7 @@
       </c>
       <c r="H163" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"162 sigilsflair syndicate-new-loka-level-8-sigil-greenGaia (New Loka) sigil (green)",</v>
+        <v>"162 sigilsflair syndicate-new-loka-level-8-sigil-green": "Gaia (New Loka) sigil (green)",</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.35">
@@ -4574,6 +4613,9 @@
       <c r="C164" s="1" t="s">
         <v>189</v>
       </c>
+      <c r="D164" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E164" s="1" t="s">
         <v>305</v>
       </c>
@@ -4582,7 +4624,7 @@
       </c>
       <c r="H164" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"163 sigilsflair syndicate-new-loka-level-9-sigil-greenBounty (New Loka) sigil (green)",</v>
+        <v>"163 sigilsflair syndicate-new-loka-level-9-sigil-green": "Bounty (New Loka) sigil (green)",</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.35">
@@ -4595,6 +4637,9 @@
       <c r="C165" s="1" t="s">
         <v>190</v>
       </c>
+      <c r="D165" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E165" s="1" t="s">
         <v>306</v>
       </c>
@@ -4603,7 +4648,7 @@
       </c>
       <c r="H165" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"164 sigilsflair syndicate-new-loka-level-10-sigil-greenHumanity (New Loka) sigil (green)",</v>
+        <v>"164 sigilsflair syndicate-new-loka-level-10-sigil-green": "Humanity (New Loka) sigil (green)",</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.35">
@@ -4616,6 +4661,9 @@
       <c r="C166" s="1" t="s">
         <v>191</v>
       </c>
+      <c r="D166" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E166" s="1" t="s">
         <v>307</v>
       </c>
@@ -4624,7 +4672,7 @@
       </c>
       <c r="H166" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"165 sigilsflair syndicate-red-veil-sigil-redRed Veil sigil (red)",</v>
+        <v>"165 sigilsflair syndicate-red-veil-sigil-red": "Red Veil sigil (red)",</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.35">
@@ -4637,6 +4685,9 @@
       <c r="C167" s="1" t="s">
         <v>192</v>
       </c>
+      <c r="D167" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E167" s="1" t="s">
         <v>308</v>
       </c>
@@ -4645,7 +4696,7 @@
       </c>
       <c r="H167" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"166 sigilsflair syndicate-red-veil-level-1-sigil-redBlades (Red Veil) sigil (red)",</v>
+        <v>"166 sigilsflair syndicate-red-veil-level-1-sigil-red": "Blades (Red Veil) sigil (red)",</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.35">
@@ -4658,6 +4709,9 @@
       <c r="C168" s="1" t="s">
         <v>193</v>
       </c>
+      <c r="D168" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E168" s="1" t="s">
         <v>309</v>
       </c>
@@ -4666,7 +4720,7 @@
       </c>
       <c r="H168" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"167 sigilsflair syndicate-red-veil-level-2-sigil-redCull (Red Veil) sigil (red)",</v>
+        <v>"167 sigilsflair syndicate-red-veil-level-2-sigil-red": "Cull (Red Veil) sigil (red)",</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.35">
@@ -4679,6 +4733,9 @@
       <c r="C169" s="1" t="s">
         <v>194</v>
       </c>
+      <c r="D169" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E169" s="1" t="s">
         <v>310</v>
       </c>
@@ -4687,7 +4744,7 @@
       </c>
       <c r="H169" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"168 sigilsflair syndicate-red-veil-level-3-sigil-redThreat (Red Veil) sigil (red)",</v>
+        <v>"168 sigilsflair syndicate-red-veil-level-3-sigil-red": "Threat (Red Veil) sigil (red)",</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.35">
@@ -4700,6 +4757,9 @@
       <c r="C170" s="1" t="s">
         <v>195</v>
       </c>
+      <c r="D170" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E170" s="1" t="s">
         <v>311</v>
       </c>
@@ -4708,7 +4768,7 @@
       </c>
       <c r="H170" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"169 sigilsflair syndicate-red-veil-level-4-sigil-redMaelstrom (Red Veil) sigil (red)",</v>
+        <v>"169 sigilsflair syndicate-red-veil-level-4-sigil-red": "Maelstrom (Red Veil) sigil (red)",</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.35">
@@ -4721,6 +4781,9 @@
       <c r="C171" s="1" t="s">
         <v>196</v>
       </c>
+      <c r="D171" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E171" s="1" t="s">
         <v>312</v>
       </c>
@@ -4729,7 +4792,7 @@
       </c>
       <c r="H171" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"170 sigilsflair syndicate-red-veil-level-5-sigil-redLesion (Red Veil) sigil (red)",</v>
+        <v>"170 sigilsflair syndicate-red-veil-level-5-sigil-red": "Lesion (Red Veil) sigil (red)",</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.35">
@@ -4742,6 +4805,9 @@
       <c r="C172" s="1" t="s">
         <v>197</v>
       </c>
+      <c r="D172" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E172" s="1" t="s">
         <v>313</v>
       </c>
@@ -4750,7 +4816,7 @@
       </c>
       <c r="H172" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"171 sigilsflair syndicate-red-veil-level-6-sigil-redRuin (Red Veil) sigil (red)",</v>
+        <v>"171 sigilsflair syndicate-red-veil-level-6-sigil-red": "Ruin (Red Veil) sigil (red)",</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.35">
@@ -4763,6 +4829,9 @@
       <c r="C173" s="1" t="s">
         <v>198</v>
       </c>
+      <c r="D173" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E173" s="1" t="s">
         <v>314</v>
       </c>
@@ -4771,7 +4840,7 @@
       </c>
       <c r="H173" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"172 sigilsflair syndicate-red-veil-level-7-sigil-redViscera (Red Veil) sigil (red)",</v>
+        <v>"172 sigilsflair syndicate-red-veil-level-7-sigil-red": "Viscera (Red Veil) sigil (red)",</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.35">
@@ -4784,6 +4853,9 @@
       <c r="C174" s="1" t="s">
         <v>199</v>
       </c>
+      <c r="D174" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E174" s="1" t="s">
         <v>315</v>
       </c>
@@ -4792,7 +4864,7 @@
       </c>
       <c r="H174" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"173 sigilsflair syndicate-red-veil-level-8-sigil-redMalevolent (Red Veil) sigil (red)",</v>
+        <v>"173 sigilsflair syndicate-red-veil-level-8-sigil-red": "Malevolent (Red Veil) sigil (red)",</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.35">
@@ -4805,6 +4877,9 @@
       <c r="C175" s="1" t="s">
         <v>200</v>
       </c>
+      <c r="D175" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E175" s="1" t="s">
         <v>316</v>
       </c>
@@ -4813,7 +4888,7 @@
       </c>
       <c r="H175" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"174 sigilsflair syndicate-red-veil-level-9-sigil-redCovert (Red Veil) sigil (red)",</v>
+        <v>"174 sigilsflair syndicate-red-veil-level-9-sigil-red": "Covert (Red Veil) sigil (red)",</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.35">
@@ -4826,6 +4901,9 @@
       <c r="C176" s="1" t="s">
         <v>201</v>
       </c>
+      <c r="D176" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E176" s="1" t="s">
         <v>317</v>
       </c>
@@ -4834,7 +4912,7 @@
       </c>
       <c r="H176" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"175 sigilsflair syndicate-red-veil-level-10-sigil-redAssassin (Red Veil) sigil (red)",</v>
+        <v>"175 sigilsflair syndicate-red-veil-level-10-sigil-red": "Assassin (Red Veil) sigil (red)",</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.35">
@@ -4847,6 +4925,9 @@
       <c r="C177" s="1" t="s">
         <v>202</v>
       </c>
+      <c r="D177" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E177" s="1" t="s">
         <v>318</v>
       </c>
@@ -4855,7 +4936,7 @@
       </c>
       <c r="H177" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"176 sigilsflair syndicate-steel-meridian-sigil-orangeSteel Meridian sigil (orange)",</v>
+        <v>"176 sigilsflair syndicate-steel-meridian-sigil-orange": "Steel Meridian sigil (orange)",</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.35">
@@ -4868,6 +4949,9 @@
       <c r="C178" s="1" t="s">
         <v>203</v>
       </c>
+      <c r="D178" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E178" s="1" t="s">
         <v>319</v>
       </c>
@@ -4876,7 +4960,7 @@
       </c>
       <c r="H178" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"177 sigilsflair syndicate-steel-meridian-level-1-sigil-orangeDefiance (Steel Meridian) sigil (orange)",</v>
+        <v>"177 sigilsflair syndicate-steel-meridian-level-1-sigil-orange": "Defiance (Steel Meridian) sigil (orange)",</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.35">
@@ -4889,6 +4973,9 @@
       <c r="C179" s="1" t="s">
         <v>204</v>
       </c>
+      <c r="D179" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E179" s="1" t="s">
         <v>320</v>
       </c>
@@ -4897,7 +4984,7 @@
       </c>
       <c r="H179" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"178 sigilsflair syndicate-steel-meridian-level-2-sigil-orangeArmada (Steel Meridian) sigil (orange)",</v>
+        <v>"178 sigilsflair syndicate-steel-meridian-level-2-sigil-orange": "Armada (Steel Meridian) sigil (orange)",</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.35">
@@ -4910,6 +4997,9 @@
       <c r="C180" s="1" t="s">
         <v>205</v>
       </c>
+      <c r="D180" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E180" s="1" t="s">
         <v>321</v>
       </c>
@@ -4918,7 +5008,7 @@
       </c>
       <c r="H180" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"179 sigilsflair syndicate-steel-meridian-level-3-sigil-orangeVigilance (Steel Meridian) sigil (orange)",</v>
+        <v>"179 sigilsflair syndicate-steel-meridian-level-3-sigil-orange": "Vigilance (Steel Meridian) sigil (orange)",</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.35">
@@ -4931,6 +5021,9 @@
       <c r="C181" s="1" t="s">
         <v>206</v>
       </c>
+      <c r="D181" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E181" s="1" t="s">
         <v>322</v>
       </c>
@@ -4939,7 +5032,7 @@
       </c>
       <c r="H181" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"180 sigilsflair syndicate-steel-meridian-level-4-sigil-orangeUprising (Steel Meridian) sigil (orange)",</v>
+        <v>"180 sigilsflair syndicate-steel-meridian-level-4-sigil-orange": "Uprising (Steel Meridian) sigil (orange)",</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.35">
@@ -4952,6 +5045,9 @@
       <c r="C182" s="1" t="s">
         <v>207</v>
       </c>
+      <c r="D182" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E182" s="1" t="s">
         <v>323</v>
       </c>
@@ -4960,7 +5056,7 @@
       </c>
       <c r="H182" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"181 sigilsflair syndicate-steel-meridian-level-5-sigil-orangeProtectorate (Steel Meridian) sigil (orange)",</v>
+        <v>"181 sigilsflair syndicate-steel-meridian-level-5-sigil-orange": "Protectorate (Steel Meridian) sigil (orange)",</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.35">
@@ -4973,6 +5069,9 @@
       <c r="C183" s="1" t="s">
         <v>208</v>
       </c>
+      <c r="D183" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E183" s="1" t="s">
         <v>324</v>
       </c>
@@ -4981,7 +5080,7 @@
       </c>
       <c r="H183" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"182 sigilsflair syndicate-steel-meridian-level-6-sigil-orangeFreedom Fighter (Steel Meridian) sigil (orange)",</v>
+        <v>"182 sigilsflair syndicate-steel-meridian-level-6-sigil-orange": "Freedom Fighter (Steel Meridian) sigil (orange)",</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.35">
@@ -4994,6 +5093,9 @@
       <c r="C184" s="1" t="s">
         <v>209</v>
       </c>
+      <c r="D184" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E184" s="1" t="s">
         <v>325</v>
       </c>
@@ -5002,7 +5104,7 @@
       </c>
       <c r="H184" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"183 sigilsflair syndicate-steel-meridian-level-7-sigil-orangeArmored (Steel Meridian) sigil (orange)",</v>
+        <v>"183 sigilsflair syndicate-steel-meridian-level-7-sigil-orange": "Armored (Steel Meridian) sigil (orange)",</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.35">
@@ -5015,6 +5117,9 @@
       <c r="C185" s="1" t="s">
         <v>210</v>
       </c>
+      <c r="D185" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E185" s="1" t="s">
         <v>326</v>
       </c>
@@ -5023,7 +5128,7 @@
       </c>
       <c r="H185" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"184 sigilsflair syndicate-steel-meridian-level-8-sigil-orangeRebellion (Steel Meridian) sigil (orange)",</v>
+        <v>"184 sigilsflair syndicate-steel-meridian-level-8-sigil-orange": "Rebellion (Steel Meridian) sigil (orange)",</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.35">
@@ -5036,6 +5141,9 @@
       <c r="C186" s="1" t="s">
         <v>211</v>
       </c>
+      <c r="D186" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E186" s="1" t="s">
         <v>327</v>
       </c>
@@ -5044,7 +5152,7 @@
       </c>
       <c r="H186" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"185 sigilsflair syndicate-steel-meridian-level-9-sigil-orangeUnyielding (Steel Meridian) sigil (orange)",</v>
+        <v>"185 sigilsflair syndicate-steel-meridian-level-9-sigil-orange": "Unyielding (Steel Meridian) sigil (orange)",</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.35">
@@ -5057,6 +5165,9 @@
       <c r="C187" s="1" t="s">
         <v>212</v>
       </c>
+      <c r="D187" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E187" s="1" t="s">
         <v>328</v>
       </c>
@@ -5065,7 +5176,7 @@
       </c>
       <c r="H187" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"186 sigilsflair syndicate-steel-meridian-level-10-sigil-orangeChampion (Steel Meridian) sigil (orange)",</v>
+        <v>"186 sigilsflair syndicate-steel-meridian-level-10-sigil-orange": "Champion (Steel Meridian) sigil (orange)",</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.35">
@@ -5078,6 +5189,9 @@
       <c r="C188" s="1" t="s">
         <v>213</v>
       </c>
+      <c r="D188" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E188" s="1" t="s">
         <v>329</v>
       </c>
@@ -5086,7 +5200,7 @@
       </c>
       <c r="H188" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"187 sigilsflair syndicate-the-perrin-sequence-sigil-blueThe Perrin Sequence sigil (blue)",</v>
+        <v>"187 sigilsflair syndicate-the-perrin-sequence-sigil-blue": "The Perrin Sequence sigil (blue)",</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.35">
@@ -5099,6 +5213,9 @@
       <c r="C189" s="1" t="s">
         <v>214</v>
       </c>
+      <c r="D189" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E189" s="1" t="s">
         <v>330</v>
       </c>
@@ -5107,7 +5224,7 @@
       </c>
       <c r="H189" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"188 sigilsflair syndicate-the-perrin-sequence-level-1-sigil-blueProgress (The Perrin Sequence) sigil (blue)",</v>
+        <v>"188 sigilsflair syndicate-the-perrin-sequence-level-1-sigil-blue": "Progress (The Perrin Sequence) sigil (blue)",</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.35">
@@ -5120,6 +5237,9 @@
       <c r="C190" s="1" t="s">
         <v>215</v>
       </c>
+      <c r="D190" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E190" s="1" t="s">
         <v>331</v>
       </c>
@@ -5128,7 +5248,7 @@
       </c>
       <c r="H190" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"189 sigilsflair syndicate-the-perrin-sequence-level-2-sigil-blueOpportunity (The Perrin Sequence) sigil (blue)",</v>
+        <v>"189 sigilsflair syndicate-the-perrin-sequence-level-2-sigil-blue": "Opportunity (The Perrin Sequence) sigil (blue)",</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.35">
@@ -5141,6 +5261,9 @@
       <c r="C191" s="1" t="s">
         <v>216</v>
       </c>
+      <c r="D191" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E191" s="1" t="s">
         <v>332</v>
       </c>
@@ -5149,7 +5272,7 @@
       </c>
       <c r="H191" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"190 sigilsflair syndicate-the-perrin-sequence-level-3-sigil-blueCalculating (The Perrin Sequence) sigil (blue)",</v>
+        <v>"190 sigilsflair syndicate-the-perrin-sequence-level-3-sigil-blue": "Calculating (The Perrin Sequence) sigil (blue)",</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.35">
@@ -5162,6 +5285,9 @@
       <c r="C192" s="1" t="s">
         <v>217</v>
       </c>
+      <c r="D192" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E192" s="1" t="s">
         <v>333</v>
       </c>
@@ -5170,7 +5296,7 @@
       </c>
       <c r="H192" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"191 sigilsflair syndicate-the-perrin-sequence-level-4-sigil-blueSynergy (The Perrin Sequence) sigil (blue)",</v>
+        <v>"191 sigilsflair syndicate-the-perrin-sequence-level-4-sigil-blue": "Synergy (The Perrin Sequence) sigil (blue)",</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.35">
@@ -5183,6 +5309,9 @@
       <c r="C193" s="1" t="s">
         <v>218</v>
       </c>
+      <c r="D193" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E193" s="1" t="s">
         <v>334</v>
       </c>
@@ -5191,7 +5320,7 @@
       </c>
       <c r="H193" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>"192 sigilsflair syndicate-the-perrin-sequence-level-5-sigil-blueDirectives (The Perrin Sequence) sigil (blue)",</v>
+        <v>"192 sigilsflair syndicate-the-perrin-sequence-level-5-sigil-blue": "Directives (The Perrin Sequence) sigil (blue)",</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.35">
@@ -5204,6 +5333,9 @@
       <c r="C194" s="1" t="s">
         <v>219</v>
       </c>
+      <c r="D194" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E194" s="1" t="s">
         <v>335</v>
       </c>
@@ -5211,8 +5343,8 @@
         <v>105</v>
       </c>
       <c r="H194" s="1" t="str">
-        <f t="shared" ref="H194:H198" si="3">A194&amp;B194&amp;C194&amp;D194&amp;E194&amp;F194</f>
-        <v>"193 sigilsflair syndicate-the-perrin-sequence-level-6-sigil-blueStrategy (The Perrin Sequence) sigil (blue)",</v>
+        <f t="shared" ref="H194:H200" si="3">A194&amp;B194&amp;C194&amp;D194&amp;E194&amp;F194</f>
+        <v>"193 sigilsflair syndicate-the-perrin-sequence-level-6-sigil-blue": "Strategy (The Perrin Sequence) sigil (blue)",</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.35">
@@ -5225,6 +5357,9 @@
       <c r="C195" s="1" t="s">
         <v>220</v>
       </c>
+      <c r="D195" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E195" s="1" t="s">
         <v>336</v>
       </c>
@@ -5233,7 +5368,7 @@
       </c>
       <c r="H195" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>"194 sigilsflair syndicate-the-perrin-sequence-level-7-sigil-blueTessilations [sic] (The Perrin Sequence) sigil (blue)",</v>
+        <v>"194 sigilsflair syndicate-the-perrin-sequence-level-7-sigil-blue": "Tessilations [sic] (The Perrin Sequence) sigil (blue)",</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.35">
@@ -5246,6 +5381,9 @@
       <c r="C196" s="1" t="s">
         <v>221</v>
       </c>
+      <c r="D196" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E196" s="1" t="s">
         <v>337</v>
       </c>
@@ -5254,7 +5392,7 @@
       </c>
       <c r="H196" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>"195 sigilsflair syndicate-the-perrin-sequence-level-8-sigil-blueOptimum (The Perrin Sequence) sigil (blue)",</v>
+        <v>"195 sigilsflair syndicate-the-perrin-sequence-level-8-sigil-blue": "Optimum (The Perrin Sequence) sigil (blue)",</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.35">
@@ -5267,6 +5405,9 @@
       <c r="C197" s="1" t="s">
         <v>222</v>
       </c>
+      <c r="D197" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E197" s="1" t="s">
         <v>338</v>
       </c>
@@ -5275,7 +5416,7 @@
       </c>
       <c r="H197" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>"196 sigilsflair syndicate-the-perrin-sequence-level-9-sigil-blueCapital (The Perrin Sequence) sigil (blue)",</v>
+        <v>"196 sigilsflair syndicate-the-perrin-sequence-level-9-sigil-blue": "Capital (The Perrin Sequence) sigil (blue)",</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.35">
@@ -5288,6 +5429,9 @@
       <c r="C198" s="1" t="s">
         <v>223</v>
       </c>
+      <c r="D198" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="E198" s="1" t="s">
         <v>339</v>
       </c>
@@ -5296,7 +5440,7 @@
       </c>
       <c r="H198" s="1" t="str">
         <f t="shared" si="3"/>
-        <v>"197 sigilsflair syndicate-the-perrin-sequence-level-10-sigil-blueChairman (The Perrin Sequence) sigil (blue)",</v>
+        <v>"197 sigilsflair syndicate-the-perrin-sequence-level-10-sigil-blue": "Chairman (The Perrin Sequence) sigil (blue)",</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.35">
@@ -5306,12 +5450,15 @@
       <c r="B199" s="1" t="s">
         <v>157</v>
       </c>
+      <c r="D199" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="F199" s="1" t="s">
         <v>105</v>
       </c>
       <c r="H199" s="1" t="str">
-        <f t="shared" ref="H199:H200" si="4">A199&amp;B199&amp;C199&amp;D199&amp;E199&amp;F199</f>
-        <v>"198 sigilsflair ",</v>
+        <f t="shared" si="3"/>
+        <v>"198 sigilsflair ": "",</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.35">
@@ -5321,12 +5468,15 @@
       <c r="B200" s="1" t="s">
         <v>157</v>
       </c>
+      <c r="D200" s="1" t="s">
+        <v>106</v>
+      </c>
       <c r="F200" s="1" t="s">
         <v>105</v>
       </c>
       <c r="H200" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>"199 sigilsflair ",</v>
+        <f t="shared" si="3"/>
+        <v>"199 sigilsflair ": "",</v>
       </c>
     </row>
   </sheetData>
@@ -5339,7 +5489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A182" workbookViewId="0">
+    <sheetView topLeftCell="A182" workbookViewId="0">
       <selection activeCell="K1" sqref="K1:K200"/>
     </sheetView>
   </sheetViews>
@@ -6009,7 +6159,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="4">
-        <f>H15-30</f>
+        <f t="shared" ref="H20:H51" si="1">H15-30</f>
         <v>-90</v>
       </c>
       <c r="I20" s="1" t="s">
@@ -6043,7 +6193,7 @@
         <v>0</v>
       </c>
       <c r="H21" s="4">
-        <f>H16-30</f>
+        <f t="shared" si="1"/>
         <v>-120</v>
       </c>
       <c r="I21" s="1" t="s">
@@ -6077,7 +6227,7 @@
         <v>0</v>
       </c>
       <c r="H22" s="4">
-        <f>H17-30</f>
+        <f t="shared" si="1"/>
         <v>-120</v>
       </c>
       <c r="I22" s="1" t="s">
@@ -6111,7 +6261,7 @@
         <v>0</v>
       </c>
       <c r="H23" s="4">
-        <f>H18-30</f>
+        <f t="shared" si="1"/>
         <v>-120</v>
       </c>
       <c r="I23" s="1" t="s">
@@ -6145,7 +6295,7 @@
         <v>0</v>
       </c>
       <c r="H24" s="4">
-        <f>H19-30</f>
+        <f t="shared" si="1"/>
         <v>-120</v>
       </c>
       <c r="I24" s="1" t="s">
@@ -6179,7 +6329,7 @@
         <v>0</v>
       </c>
       <c r="H25" s="4">
-        <f>H20-30</f>
+        <f t="shared" si="1"/>
         <v>-120</v>
       </c>
       <c r="I25" s="1" t="s">
@@ -6213,7 +6363,7 @@
         <v>0</v>
       </c>
       <c r="H26" s="4">
-        <f>H21-30</f>
+        <f t="shared" si="1"/>
         <v>-150</v>
       </c>
       <c r="I26" s="1" t="s">
@@ -6247,7 +6397,7 @@
         <v>0</v>
       </c>
       <c r="H27" s="4">
-        <f>H22-30</f>
+        <f t="shared" si="1"/>
         <v>-150</v>
       </c>
       <c r="I27" s="1" t="s">
@@ -6281,7 +6431,7 @@
         <v>0</v>
       </c>
       <c r="H28" s="4">
-        <f>H23-30</f>
+        <f t="shared" si="1"/>
         <v>-150</v>
       </c>
       <c r="I28" s="1" t="s">
@@ -6315,7 +6465,7 @@
         <v>0</v>
       </c>
       <c r="H29" s="4">
-        <f>H24-30</f>
+        <f t="shared" si="1"/>
         <v>-150</v>
       </c>
       <c r="I29" s="1" t="s">
@@ -6349,7 +6499,7 @@
         <v>0</v>
       </c>
       <c r="H30" s="4">
-        <f>H25-30</f>
+        <f t="shared" si="1"/>
         <v>-150</v>
       </c>
       <c r="I30" s="1" t="s">
@@ -6383,7 +6533,7 @@
         <v>0</v>
       </c>
       <c r="H31" s="4">
-        <f>H26-30</f>
+        <f t="shared" si="1"/>
         <v>-180</v>
       </c>
       <c r="I31" s="1" t="s">
@@ -6417,7 +6567,7 @@
         <v>0</v>
       </c>
       <c r="H32" s="4">
-        <f>H27-30</f>
+        <f t="shared" si="1"/>
         <v>-180</v>
       </c>
       <c r="I32" s="1" t="s">
@@ -6451,7 +6601,7 @@
         <v>0</v>
       </c>
       <c r="H33" s="4">
-        <f>H28-30</f>
+        <f t="shared" si="1"/>
         <v>-180</v>
       </c>
       <c r="I33" s="1" t="s">
@@ -6485,7 +6635,7 @@
         <v>0</v>
       </c>
       <c r="H34" s="4">
-        <f>H29-30</f>
+        <f t="shared" si="1"/>
         <v>-180</v>
       </c>
       <c r="I34" s="1" t="s">
@@ -6519,7 +6669,7 @@
         <v>0</v>
       </c>
       <c r="H35" s="4">
-        <f>H30-30</f>
+        <f t="shared" si="1"/>
         <v>-180</v>
       </c>
       <c r="I35" s="1" t="s">
@@ -6553,7 +6703,7 @@
         <v>0</v>
       </c>
       <c r="H36" s="4">
-        <f>H31-30</f>
+        <f t="shared" si="1"/>
         <v>-210</v>
       </c>
       <c r="I36" s="1" t="s">
@@ -6587,7 +6737,7 @@
         <v>0</v>
       </c>
       <c r="H37" s="4">
-        <f>H32-30</f>
+        <f t="shared" si="1"/>
         <v>-210</v>
       </c>
       <c r="I37" s="1" t="s">
@@ -6621,7 +6771,7 @@
         <v>0</v>
       </c>
       <c r="H38" s="4">
-        <f>H33-30</f>
+        <f t="shared" si="1"/>
         <v>-210</v>
       </c>
       <c r="I38" s="1" t="s">
@@ -6655,7 +6805,7 @@
         <v>0</v>
       </c>
       <c r="H39" s="4">
-        <f>H34-30</f>
+        <f t="shared" si="1"/>
         <v>-210</v>
       </c>
       <c r="I39" s="1" t="s">
@@ -6689,7 +6839,7 @@
         <v>0</v>
       </c>
       <c r="H40" s="4">
-        <f>H35-30</f>
+        <f t="shared" si="1"/>
         <v>-210</v>
       </c>
       <c r="I40" s="1" t="s">
@@ -6723,7 +6873,7 @@
         <v>0</v>
       </c>
       <c r="H41" s="4">
-        <f>H36-30</f>
+        <f t="shared" si="1"/>
         <v>-240</v>
       </c>
       <c r="I41" s="1" t="s">
@@ -6757,7 +6907,7 @@
         <v>0</v>
       </c>
       <c r="H42" s="4">
-        <f>H37-30</f>
+        <f t="shared" si="1"/>
         <v>-240</v>
       </c>
       <c r="I42" s="1" t="s">
@@ -6791,7 +6941,7 @@
         <v>0</v>
       </c>
       <c r="H43" s="4">
-        <f>H38-30</f>
+        <f t="shared" si="1"/>
         <v>-240</v>
       </c>
       <c r="I43" s="1" t="s">
@@ -6825,7 +6975,7 @@
         <v>0</v>
       </c>
       <c r="H44" s="4">
-        <f>H39-30</f>
+        <f t="shared" si="1"/>
         <v>-240</v>
       </c>
       <c r="I44" s="1" t="s">
@@ -6859,7 +7009,7 @@
         <v>0</v>
       </c>
       <c r="H45" s="4">
-        <f>H40-30</f>
+        <f t="shared" si="1"/>
         <v>-240</v>
       </c>
       <c r="I45" s="1" t="s">
@@ -6893,7 +7043,7 @@
         <v>0</v>
       </c>
       <c r="H46" s="4">
-        <f>H41-30</f>
+        <f t="shared" si="1"/>
         <v>-270</v>
       </c>
       <c r="I46" s="1" t="s">
@@ -6927,7 +7077,7 @@
         <v>0</v>
       </c>
       <c r="H47" s="4">
-        <f>H42-30</f>
+        <f t="shared" si="1"/>
         <v>-270</v>
       </c>
       <c r="I47" s="1" t="s">
@@ -6961,7 +7111,7 @@
         <v>0</v>
       </c>
       <c r="H48" s="4">
-        <f>H43-30</f>
+        <f t="shared" si="1"/>
         <v>-270</v>
       </c>
       <c r="I48" s="1" t="s">
@@ -6995,7 +7145,7 @@
         <v>0</v>
       </c>
       <c r="H49" s="4">
-        <f>H44-30</f>
+        <f t="shared" si="1"/>
         <v>-270</v>
       </c>
       <c r="I49" s="1" t="s">
@@ -7029,7 +7179,7 @@
         <v>0</v>
       </c>
       <c r="H50" s="4">
-        <f>H45-30</f>
+        <f t="shared" si="1"/>
         <v>-270</v>
       </c>
       <c r="I50" s="1" t="s">
@@ -7063,7 +7213,7 @@
         <v>0</v>
       </c>
       <c r="H51" s="4">
-        <f>H46-30</f>
+        <f t="shared" si="1"/>
         <v>-300</v>
       </c>
       <c r="I51" s="1" t="s">
@@ -7097,7 +7247,7 @@
         <v>0</v>
       </c>
       <c r="H52" s="4">
-        <f>H47-30</f>
+        <f t="shared" ref="H52:H83" si="2">H47-30</f>
         <v>-300</v>
       </c>
       <c r="I52" s="1" t="s">
@@ -7131,7 +7281,7 @@
         <v>0</v>
       </c>
       <c r="H53" s="4">
-        <f>H48-30</f>
+        <f t="shared" si="2"/>
         <v>-300</v>
       </c>
       <c r="I53" s="1" t="s">
@@ -7165,7 +7315,7 @@
         <v>0</v>
       </c>
       <c r="H54" s="4">
-        <f>H49-30</f>
+        <f t="shared" si="2"/>
         <v>-300</v>
       </c>
       <c r="I54" s="1" t="s">
@@ -7199,7 +7349,7 @@
         <v>0</v>
       </c>
       <c r="H55" s="4">
-        <f>H50-30</f>
+        <f t="shared" si="2"/>
         <v>-300</v>
       </c>
       <c r="I55" s="1" t="s">
@@ -7233,7 +7383,7 @@
         <v>0</v>
       </c>
       <c r="H56" s="4">
-        <f>H51-30</f>
+        <f t="shared" si="2"/>
         <v>-330</v>
       </c>
       <c r="I56" s="1" t="s">
@@ -7267,7 +7417,7 @@
         <v>0</v>
       </c>
       <c r="H57" s="4">
-        <f>H52-30</f>
+        <f t="shared" si="2"/>
         <v>-330</v>
       </c>
       <c r="I57" s="1" t="s">
@@ -7301,7 +7451,7 @@
         <v>0</v>
       </c>
       <c r="H58" s="4">
-        <f>H53-30</f>
+        <f t="shared" si="2"/>
         <v>-330</v>
       </c>
       <c r="I58" s="1" t="s">
@@ -7335,7 +7485,7 @@
         <v>0</v>
       </c>
       <c r="H59" s="4">
-        <f>H54-30</f>
+        <f t="shared" si="2"/>
         <v>-330</v>
       </c>
       <c r="I59" s="1" t="s">
@@ -7369,7 +7519,7 @@
         <v>0</v>
       </c>
       <c r="H60" s="4">
-        <f>H55-30</f>
+        <f t="shared" si="2"/>
         <v>-330</v>
       </c>
       <c r="I60" s="1" t="s">
@@ -7403,7 +7553,7 @@
         <v>0</v>
       </c>
       <c r="H61" s="4">
-        <f>H56-30</f>
+        <f t="shared" si="2"/>
         <v>-360</v>
       </c>
       <c r="I61" s="1" t="s">
@@ -7437,7 +7587,7 @@
         <v>0</v>
       </c>
       <c r="H62" s="4">
-        <f>H57-30</f>
+        <f t="shared" si="2"/>
         <v>-360</v>
       </c>
       <c r="I62" s="1" t="s">
@@ -7471,7 +7621,7 @@
         <v>0</v>
       </c>
       <c r="H63" s="4">
-        <f>H58-30</f>
+        <f t="shared" si="2"/>
         <v>-360</v>
       </c>
       <c r="I63" s="1" t="s">
@@ -7505,7 +7655,7 @@
         <v>0</v>
       </c>
       <c r="H64" s="4">
-        <f>H59-30</f>
+        <f t="shared" si="2"/>
         <v>-360</v>
       </c>
       <c r="I64" s="1" t="s">
@@ -7539,7 +7689,7 @@
         <v>0</v>
       </c>
       <c r="H65" s="4">
-        <f>H60-30</f>
+        <f t="shared" si="2"/>
         <v>-360</v>
       </c>
       <c r="I65" s="1" t="s">
@@ -7573,14 +7723,14 @@
         <v>0</v>
       </c>
       <c r="H66" s="4">
-        <f>H61-30</f>
+        <f t="shared" si="2"/>
         <v>-390</v>
       </c>
       <c r="I66" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K66" s="1" t="str">
-        <f t="shared" ref="K66:K129" si="1">A66&amp;B66&amp;C66&amp;D66&amp;E66&amp;F66&amp;G66&amp;H66&amp;I66</f>
+        <f t="shared" ref="K66:K129" si="3">A66&amp;B66&amp;C66&amp;D66&amp;E66&amp;F66&amp;G66&amp;H66&amp;I66</f>
         <v>.flair-65 { background: 0px -390px; }</v>
       </c>
     </row>
@@ -7607,14 +7757,14 @@
         <v>0</v>
       </c>
       <c r="H67" s="4">
-        <f>H62-30</f>
+        <f t="shared" si="2"/>
         <v>-390</v>
       </c>
       <c r="I67" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K67" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-66 { background: -0047px -390px; }</v>
       </c>
     </row>
@@ -7641,14 +7791,14 @@
         <v>0</v>
       </c>
       <c r="H68" s="4">
-        <f>H63-30</f>
+        <f t="shared" si="2"/>
         <v>-390</v>
       </c>
       <c r="I68" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K68" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-67 { background: -0094px -390px; }</v>
       </c>
     </row>
@@ -7675,14 +7825,14 @@
         <v>0</v>
       </c>
       <c r="H69" s="4">
-        <f>H64-30</f>
+        <f t="shared" si="2"/>
         <v>-390</v>
       </c>
       <c r="I69" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K69" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-68 { background: -0141px -390px; }</v>
       </c>
     </row>
@@ -7709,14 +7859,14 @@
         <v>0</v>
       </c>
       <c r="H70" s="4">
-        <f>H65-30</f>
+        <f t="shared" si="2"/>
         <v>-390</v>
       </c>
       <c r="I70" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K70" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-69 { background: -0188px -390px; }</v>
       </c>
     </row>
@@ -7743,14 +7893,14 @@
         <v>0</v>
       </c>
       <c r="H71" s="4">
-        <f>H66-30</f>
+        <f t="shared" si="2"/>
         <v>-420</v>
       </c>
       <c r="I71" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K71" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-70 { background: 0px -420px; }</v>
       </c>
     </row>
@@ -7777,14 +7927,14 @@
         <v>0</v>
       </c>
       <c r="H72" s="4">
-        <f>H67-30</f>
+        <f t="shared" si="2"/>
         <v>-420</v>
       </c>
       <c r="I72" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K72" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-71 { background: -0047px -420px; }</v>
       </c>
     </row>
@@ -7811,14 +7961,14 @@
         <v>0</v>
       </c>
       <c r="H73" s="4">
-        <f>H68-30</f>
+        <f t="shared" si="2"/>
         <v>-420</v>
       </c>
       <c r="I73" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K73" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-72 { background: -0094px -420px; }</v>
       </c>
     </row>
@@ -7845,14 +7995,14 @@
         <v>0</v>
       </c>
       <c r="H74" s="4">
-        <f>H69-30</f>
+        <f t="shared" si="2"/>
         <v>-420</v>
       </c>
       <c r="I74" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K74" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-73 { background: -0141px -420px; }</v>
       </c>
     </row>
@@ -7879,14 +8029,14 @@
         <v>0</v>
       </c>
       <c r="H75" s="4">
-        <f>H70-30</f>
+        <f t="shared" si="2"/>
         <v>-420</v>
       </c>
       <c r="I75" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K75" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-74 { background: -0188px -420px; }</v>
       </c>
     </row>
@@ -7913,14 +8063,14 @@
         <v>0</v>
       </c>
       <c r="H76" s="4">
-        <f>H71-30</f>
+        <f t="shared" si="2"/>
         <v>-450</v>
       </c>
       <c r="I76" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K76" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-75 { background: 0px -450px; }</v>
       </c>
     </row>
@@ -7947,14 +8097,14 @@
         <v>0</v>
       </c>
       <c r="H77" s="4">
-        <f>H72-30</f>
+        <f t="shared" si="2"/>
         <v>-450</v>
       </c>
       <c r="I77" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K77" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-76 { background: -0047px -450px; }</v>
       </c>
     </row>
@@ -7981,14 +8131,14 @@
         <v>0</v>
       </c>
       <c r="H78" s="4">
-        <f>H73-30</f>
+        <f t="shared" si="2"/>
         <v>-450</v>
       </c>
       <c r="I78" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K78" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-77 { background: -0094px -450px; }</v>
       </c>
     </row>
@@ -8015,14 +8165,14 @@
         <v>0</v>
       </c>
       <c r="H79" s="4">
-        <f>H74-30</f>
+        <f t="shared" si="2"/>
         <v>-450</v>
       </c>
       <c r="I79" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K79" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-78 { background: -0141px -450px; }</v>
       </c>
     </row>
@@ -8049,14 +8199,14 @@
         <v>0</v>
       </c>
       <c r="H80" s="4">
-        <f>H75-30</f>
+        <f t="shared" si="2"/>
         <v>-450</v>
       </c>
       <c r="I80" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K80" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-79 { background: -0188px -450px; }</v>
       </c>
     </row>
@@ -8083,14 +8233,14 @@
         <v>0</v>
       </c>
       <c r="H81" s="4">
-        <f>H76-30</f>
+        <f t="shared" si="2"/>
         <v>-480</v>
       </c>
       <c r="I81" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K81" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-80 { background: 0px -480px; }</v>
       </c>
     </row>
@@ -8117,14 +8267,14 @@
         <v>0</v>
       </c>
       <c r="H82" s="4">
-        <f>H77-30</f>
+        <f t="shared" si="2"/>
         <v>-480</v>
       </c>
       <c r="I82" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K82" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-81 { background: -0047px -480px; }</v>
       </c>
     </row>
@@ -8151,14 +8301,14 @@
         <v>0</v>
       </c>
       <c r="H83" s="4">
-        <f>H78-30</f>
+        <f t="shared" si="2"/>
         <v>-480</v>
       </c>
       <c r="I83" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K83" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-82 { background: -0094px -480px; }</v>
       </c>
     </row>
@@ -8185,14 +8335,14 @@
         <v>0</v>
       </c>
       <c r="H84" s="4">
-        <f>H79-30</f>
+        <f t="shared" ref="H84:H115" si="4">H79-30</f>
         <v>-480</v>
       </c>
       <c r="I84" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K84" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-83 { background: -0141px -480px; }</v>
       </c>
     </row>
@@ -8219,14 +8369,14 @@
         <v>0</v>
       </c>
       <c r="H85" s="4">
-        <f>H80-30</f>
+        <f t="shared" si="4"/>
         <v>-480</v>
       </c>
       <c r="I85" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K85" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-84 { background: -0188px -480px; }</v>
       </c>
     </row>
@@ -8253,14 +8403,14 @@
         <v>0</v>
       </c>
       <c r="H86" s="4">
-        <f>H81-30</f>
+        <f t="shared" si="4"/>
         <v>-510</v>
       </c>
       <c r="I86" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K86" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-85 { background: 0px -510px; }</v>
       </c>
     </row>
@@ -8287,14 +8437,14 @@
         <v>0</v>
       </c>
       <c r="H87" s="4">
-        <f>H82-30</f>
+        <f t="shared" si="4"/>
         <v>-510</v>
       </c>
       <c r="I87" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K87" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-86 { background: -0047px -510px; }</v>
       </c>
     </row>
@@ -8321,14 +8471,14 @@
         <v>0</v>
       </c>
       <c r="H88" s="4">
-        <f>H83-30</f>
+        <f t="shared" si="4"/>
         <v>-510</v>
       </c>
       <c r="I88" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K88" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-87 { background: -0094px -510px; }</v>
       </c>
     </row>
@@ -8355,14 +8505,14 @@
         <v>0</v>
       </c>
       <c r="H89" s="4">
-        <f>H84-30</f>
+        <f t="shared" si="4"/>
         <v>-510</v>
       </c>
       <c r="I89" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K89" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-88 { background: -0141px -510px; }</v>
       </c>
     </row>
@@ -8389,14 +8539,14 @@
         <v>0</v>
       </c>
       <c r="H90" s="4">
-        <f>H85-30</f>
+        <f t="shared" si="4"/>
         <v>-510</v>
       </c>
       <c r="I90" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K90" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-89 { background: -0188px -510px; }</v>
       </c>
     </row>
@@ -8423,14 +8573,14 @@
         <v>0</v>
       </c>
       <c r="H91" s="4">
-        <f>H86-30</f>
+        <f t="shared" si="4"/>
         <v>-540</v>
       </c>
       <c r="I91" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K91" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-90 { background: 0px -540px; }</v>
       </c>
     </row>
@@ -8457,14 +8607,14 @@
         <v>0</v>
       </c>
       <c r="H92" s="4">
-        <f>H87-30</f>
+        <f t="shared" si="4"/>
         <v>-540</v>
       </c>
       <c r="I92" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K92" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-91 { background: -0047px -540px; }</v>
       </c>
     </row>
@@ -8491,14 +8641,14 @@
         <v>0</v>
       </c>
       <c r="H93" s="4">
-        <f>H88-30</f>
+        <f t="shared" si="4"/>
         <v>-540</v>
       </c>
       <c r="I93" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K93" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-92 { background: -0094px -540px; }</v>
       </c>
     </row>
@@ -8525,14 +8675,14 @@
         <v>0</v>
       </c>
       <c r="H94" s="4">
-        <f>H89-30</f>
+        <f t="shared" si="4"/>
         <v>-540</v>
       </c>
       <c r="I94" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K94" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-93 { background: -0141px -540px; }</v>
       </c>
     </row>
@@ -8559,14 +8709,14 @@
         <v>0</v>
       </c>
       <c r="H95" s="4">
-        <f>H90-30</f>
+        <f t="shared" si="4"/>
         <v>-540</v>
       </c>
       <c r="I95" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K95" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-94 { background: -0188px -540px; }</v>
       </c>
     </row>
@@ -8593,14 +8743,14 @@
         <v>0</v>
       </c>
       <c r="H96" s="4">
-        <f>H91-30</f>
+        <f t="shared" si="4"/>
         <v>-570</v>
       </c>
       <c r="I96" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K96" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-95 { background: 0px -570px; }</v>
       </c>
     </row>
@@ -8627,14 +8777,14 @@
         <v>0</v>
       </c>
       <c r="H97" s="4">
-        <f>H92-30</f>
+        <f t="shared" si="4"/>
         <v>-570</v>
       </c>
       <c r="I97" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K97" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-96 { background: -0047px -570px; }</v>
       </c>
     </row>
@@ -8661,14 +8811,14 @@
         <v>0</v>
       </c>
       <c r="H98" s="4">
-        <f>H93-30</f>
+        <f t="shared" si="4"/>
         <v>-570</v>
       </c>
       <c r="I98" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K98" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-97 { background: -0094px -570px; }</v>
       </c>
     </row>
@@ -8695,14 +8845,14 @@
         <v>0</v>
       </c>
       <c r="H99" s="4">
-        <f>H94-30</f>
+        <f t="shared" si="4"/>
         <v>-570</v>
       </c>
       <c r="I99" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K99" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-98 { background: -0141px -570px; }</v>
       </c>
     </row>
@@ -8729,14 +8879,14 @@
         <v>0</v>
       </c>
       <c r="H100" s="4">
-        <f>H95-30</f>
+        <f t="shared" si="4"/>
         <v>-570</v>
       </c>
       <c r="I100" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K100" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-99 { background: -0188px -570px; }</v>
       </c>
     </row>
@@ -8763,14 +8913,14 @@
         <v>0</v>
       </c>
       <c r="H101" s="4">
-        <f>H96-30</f>
+        <f t="shared" si="4"/>
         <v>-600</v>
       </c>
       <c r="I101" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K101" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-100 { background: 0px -600px; }</v>
       </c>
     </row>
@@ -8797,14 +8947,14 @@
         <v>0</v>
       </c>
       <c r="H102" s="4">
-        <f>H97-30</f>
+        <f t="shared" si="4"/>
         <v>-600</v>
       </c>
       <c r="I102" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K102" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-101 { background: -0047px -600px; }</v>
       </c>
     </row>
@@ -8831,14 +8981,14 @@
         <v>0</v>
       </c>
       <c r="H103" s="4">
-        <f>H98-30</f>
+        <f t="shared" si="4"/>
         <v>-600</v>
       </c>
       <c r="I103" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K103" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-102 { background: -0094px -600px; }</v>
       </c>
     </row>
@@ -8865,14 +9015,14 @@
         <v>0</v>
       </c>
       <c r="H104" s="4">
-        <f>H99-30</f>
+        <f t="shared" si="4"/>
         <v>-600</v>
       </c>
       <c r="I104" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K104" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-103 { background: -0141px -600px; }</v>
       </c>
     </row>
@@ -8899,14 +9049,14 @@
         <v>0</v>
       </c>
       <c r="H105" s="4">
-        <f>H100-30</f>
+        <f t="shared" si="4"/>
         <v>-600</v>
       </c>
       <c r="I105" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K105" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-104 { background: -0188px -600px; }</v>
       </c>
     </row>
@@ -8933,14 +9083,14 @@
         <v>0</v>
       </c>
       <c r="H106" s="4">
-        <f>H101-30</f>
+        <f t="shared" si="4"/>
         <v>-630</v>
       </c>
       <c r="I106" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K106" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-105 { background: 0px -630px; }</v>
       </c>
     </row>
@@ -8967,14 +9117,14 @@
         <v>0</v>
       </c>
       <c r="H107" s="4">
-        <f>H102-30</f>
+        <f t="shared" si="4"/>
         <v>-630</v>
       </c>
       <c r="I107" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K107" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-106 { background: -0047px -630px; }</v>
       </c>
     </row>
@@ -9001,14 +9151,14 @@
         <v>0</v>
       </c>
       <c r="H108" s="4">
-        <f>H103-30</f>
+        <f t="shared" si="4"/>
         <v>-630</v>
       </c>
       <c r="I108" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K108" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-107 { background: -0094px -630px; }</v>
       </c>
     </row>
@@ -9035,14 +9185,14 @@
         <v>0</v>
       </c>
       <c r="H109" s="4">
-        <f>H104-30</f>
+        <f t="shared" si="4"/>
         <v>-630</v>
       </c>
       <c r="I109" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K109" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-108 { background: -0141px -630px; }</v>
       </c>
     </row>
@@ -9069,14 +9219,14 @@
         <v>0</v>
       </c>
       <c r="H110" s="4">
-        <f>H105-30</f>
+        <f t="shared" si="4"/>
         <v>-630</v>
       </c>
       <c r="I110" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K110" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-109 { background: -0188px -630px; }</v>
       </c>
     </row>
@@ -9103,14 +9253,14 @@
         <v>0</v>
       </c>
       <c r="H111" s="4">
-        <f>H106-30</f>
+        <f t="shared" si="4"/>
         <v>-660</v>
       </c>
       <c r="I111" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K111" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-110 { background: 0px -660px; }</v>
       </c>
     </row>
@@ -9137,14 +9287,14 @@
         <v>0</v>
       </c>
       <c r="H112" s="4">
-        <f>H107-30</f>
+        <f t="shared" si="4"/>
         <v>-660</v>
       </c>
       <c r="I112" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K112" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-111 { background: -0047px -660px; }</v>
       </c>
     </row>
@@ -9171,14 +9321,14 @@
         <v>0</v>
       </c>
       <c r="H113" s="4">
-        <f>H108-30</f>
+        <f t="shared" si="4"/>
         <v>-660</v>
       </c>
       <c r="I113" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K113" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-112 { background: -0094px -660px; }</v>
       </c>
     </row>
@@ -9205,14 +9355,14 @@
         <v>0</v>
       </c>
       <c r="H114" s="4">
-        <f>H109-30</f>
+        <f t="shared" si="4"/>
         <v>-660</v>
       </c>
       <c r="I114" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K114" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-113 { background: -0141px -660px; }</v>
       </c>
     </row>
@@ -9239,14 +9389,14 @@
         <v>0</v>
       </c>
       <c r="H115" s="4">
-        <f>H110-30</f>
+        <f t="shared" si="4"/>
         <v>-660</v>
       </c>
       <c r="I115" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K115" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-114 { background: -0188px -660px; }</v>
       </c>
     </row>
@@ -9273,14 +9423,14 @@
         <v>0</v>
       </c>
       <c r="H116" s="4">
-        <f>H111-30</f>
+        <f t="shared" ref="H116:H147" si="5">H111-30</f>
         <v>-690</v>
       </c>
       <c r="I116" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K116" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-115 { background: 0px -690px; }</v>
       </c>
     </row>
@@ -9307,14 +9457,14 @@
         <v>0</v>
       </c>
       <c r="H117" s="4">
-        <f>H112-30</f>
+        <f t="shared" si="5"/>
         <v>-690</v>
       </c>
       <c r="I117" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K117" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-116 { background: -0047px -690px; }</v>
       </c>
     </row>
@@ -9341,14 +9491,14 @@
         <v>0</v>
       </c>
       <c r="H118" s="4">
-        <f>H113-30</f>
+        <f t="shared" si="5"/>
         <v>-690</v>
       </c>
       <c r="I118" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K118" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-117 { background: -0094px -690px; }</v>
       </c>
     </row>
@@ -9375,14 +9525,14 @@
         <v>0</v>
       </c>
       <c r="H119" s="4">
-        <f>H114-30</f>
+        <f t="shared" si="5"/>
         <v>-690</v>
       </c>
       <c r="I119" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K119" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-118 { background: -0141px -690px; }</v>
       </c>
     </row>
@@ -9409,14 +9559,14 @@
         <v>0</v>
       </c>
       <c r="H120" s="4">
-        <f>H115-30</f>
+        <f t="shared" si="5"/>
         <v>-690</v>
       </c>
       <c r="I120" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K120" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-119 { background: -0188px -690px; }</v>
       </c>
     </row>
@@ -9443,14 +9593,14 @@
         <v>0</v>
       </c>
       <c r="H121" s="4">
-        <f>H116-30</f>
+        <f t="shared" si="5"/>
         <v>-720</v>
       </c>
       <c r="I121" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K121" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-120 { background: 0px -720px; }</v>
       </c>
     </row>
@@ -9477,14 +9627,14 @@
         <v>0</v>
       </c>
       <c r="H122" s="4">
-        <f>H117-30</f>
+        <f t="shared" si="5"/>
         <v>-720</v>
       </c>
       <c r="I122" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K122" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-121 { background: -0047px -720px; }</v>
       </c>
     </row>
@@ -9511,14 +9661,14 @@
         <v>0</v>
       </c>
       <c r="H123" s="4">
-        <f>H118-30</f>
+        <f t="shared" si="5"/>
         <v>-720</v>
       </c>
       <c r="I123" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K123" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-122 { background: -0094px -720px; }</v>
       </c>
     </row>
@@ -9545,14 +9695,14 @@
         <v>0</v>
       </c>
       <c r="H124" s="4">
-        <f>H119-30</f>
+        <f t="shared" si="5"/>
         <v>-720</v>
       </c>
       <c r="I124" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K124" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-123 { background: -0141px -720px; }</v>
       </c>
     </row>
@@ -9579,14 +9729,14 @@
         <v>0</v>
       </c>
       <c r="H125" s="4">
-        <f>H120-30</f>
+        <f t="shared" si="5"/>
         <v>-720</v>
       </c>
       <c r="I125" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K125" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-124 { background: -0188px -720px; }</v>
       </c>
     </row>
@@ -9613,14 +9763,14 @@
         <v>0</v>
       </c>
       <c r="H126" s="4">
-        <f>H121-30</f>
+        <f t="shared" si="5"/>
         <v>-750</v>
       </c>
       <c r="I126" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K126" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-125 { background: 0px -750px; }</v>
       </c>
     </row>
@@ -9647,14 +9797,14 @@
         <v>0</v>
       </c>
       <c r="H127" s="4">
-        <f>H122-30</f>
+        <f t="shared" si="5"/>
         <v>-750</v>
       </c>
       <c r="I127" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K127" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-126 { background: -0047px -750px; }</v>
       </c>
     </row>
@@ -9681,14 +9831,14 @@
         <v>0</v>
       </c>
       <c r="H128" s="4">
-        <f>H123-30</f>
+        <f t="shared" si="5"/>
         <v>-750</v>
       </c>
       <c r="I128" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K128" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-127 { background: -0094px -750px; }</v>
       </c>
     </row>
@@ -9715,14 +9865,14 @@
         <v>0</v>
       </c>
       <c r="H129" s="4">
-        <f>H124-30</f>
+        <f t="shared" si="5"/>
         <v>-750</v>
       </c>
       <c r="I129" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K129" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>.flair-128 { background: -0141px -750px; }</v>
       </c>
     </row>
@@ -9749,14 +9899,14 @@
         <v>0</v>
       </c>
       <c r="H130" s="4">
-        <f>H125-30</f>
+        <f t="shared" si="5"/>
         <v>-750</v>
       </c>
       <c r="I130" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K130" s="1" t="str">
-        <f t="shared" ref="K130:K193" si="2">A130&amp;B130&amp;C130&amp;D130&amp;E130&amp;F130&amp;G130&amp;H130&amp;I130</f>
+        <f t="shared" ref="K130:K193" si="6">A130&amp;B130&amp;C130&amp;D130&amp;E130&amp;F130&amp;G130&amp;H130&amp;I130</f>
         <v>.flair-129 { background: -0188px -750px; }</v>
       </c>
     </row>
@@ -9783,14 +9933,14 @@
         <v>0</v>
       </c>
       <c r="H131" s="4">
-        <f>H126-30</f>
+        <f t="shared" si="5"/>
         <v>-780</v>
       </c>
       <c r="I131" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K131" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-130 { background: 0px -780px; }</v>
       </c>
     </row>
@@ -9817,14 +9967,14 @@
         <v>0</v>
       </c>
       <c r="H132" s="4">
-        <f>H127-30</f>
+        <f t="shared" si="5"/>
         <v>-780</v>
       </c>
       <c r="I132" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K132" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-131 { background: -0047px -780px; }</v>
       </c>
     </row>
@@ -9851,14 +10001,14 @@
         <v>0</v>
       </c>
       <c r="H133" s="4">
-        <f>H128-30</f>
+        <f t="shared" si="5"/>
         <v>-780</v>
       </c>
       <c r="I133" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K133" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-132 { background: -0094px -780px; }</v>
       </c>
     </row>
@@ -9885,14 +10035,14 @@
         <v>0</v>
       </c>
       <c r="H134" s="4">
-        <f>H129-30</f>
+        <f t="shared" si="5"/>
         <v>-780</v>
       </c>
       <c r="I134" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K134" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-133 { background: -0141px -780px; }</v>
       </c>
     </row>
@@ -9919,14 +10069,14 @@
         <v>0</v>
       </c>
       <c r="H135" s="4">
-        <f>H130-30</f>
+        <f t="shared" si="5"/>
         <v>-780</v>
       </c>
       <c r="I135" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K135" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-134 { background: -0188px -780px; }</v>
       </c>
     </row>
@@ -9953,14 +10103,14 @@
         <v>0</v>
       </c>
       <c r="H136" s="4">
-        <f>H131-30</f>
+        <f t="shared" si="5"/>
         <v>-810</v>
       </c>
       <c r="I136" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K136" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-135 { background: 0px -810px; }</v>
       </c>
     </row>
@@ -9987,14 +10137,14 @@
         <v>0</v>
       </c>
       <c r="H137" s="4">
-        <f>H132-30</f>
+        <f t="shared" si="5"/>
         <v>-810</v>
       </c>
       <c r="I137" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K137" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-136 { background: -0047px -810px; }</v>
       </c>
     </row>
@@ -10021,14 +10171,14 @@
         <v>0</v>
       </c>
       <c r="H138" s="4">
-        <f>H133-30</f>
+        <f t="shared" si="5"/>
         <v>-810</v>
       </c>
       <c r="I138" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K138" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-137 { background: -0094px -810px; }</v>
       </c>
     </row>
@@ -10055,14 +10205,14 @@
         <v>0</v>
       </c>
       <c r="H139" s="4">
-        <f>H134-30</f>
+        <f t="shared" si="5"/>
         <v>-810</v>
       </c>
       <c r="I139" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K139" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-138 { background: -0141px -810px; }</v>
       </c>
     </row>
@@ -10089,14 +10239,14 @@
         <v>0</v>
       </c>
       <c r="H140" s="4">
-        <f>H135-30</f>
+        <f t="shared" si="5"/>
         <v>-810</v>
       </c>
       <c r="I140" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K140" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-139 { background: -0188px -810px; }</v>
       </c>
     </row>
@@ -10123,14 +10273,14 @@
         <v>0</v>
       </c>
       <c r="H141" s="4">
-        <f>H136-30</f>
+        <f t="shared" si="5"/>
         <v>-840</v>
       </c>
       <c r="I141" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K141" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-140 { background: 0px -840px; }</v>
       </c>
     </row>
@@ -10157,14 +10307,14 @@
         <v>0</v>
       </c>
       <c r="H142" s="4">
-        <f>H137-30</f>
+        <f t="shared" si="5"/>
         <v>-840</v>
       </c>
       <c r="I142" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K142" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-141 { background: -0047px -840px; }</v>
       </c>
     </row>
@@ -10191,14 +10341,14 @@
         <v>0</v>
       </c>
       <c r="H143" s="4">
-        <f>H138-30</f>
+        <f t="shared" si="5"/>
         <v>-840</v>
       </c>
       <c r="I143" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K143" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-142 { background: -0094px -840px; }</v>
       </c>
     </row>
@@ -10225,14 +10375,14 @@
         <v>0</v>
       </c>
       <c r="H144" s="4">
-        <f>H139-30</f>
+        <f t="shared" si="5"/>
         <v>-840</v>
       </c>
       <c r="I144" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K144" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-143 { background: -0141px -840px; }</v>
       </c>
     </row>
@@ -10259,14 +10409,14 @@
         <v>0</v>
       </c>
       <c r="H145" s="4">
-        <f>H140-30</f>
+        <f t="shared" si="5"/>
         <v>-840</v>
       </c>
       <c r="I145" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K145" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-144 { background: -0188px -840px; }</v>
       </c>
     </row>
@@ -10293,14 +10443,14 @@
         <v>0</v>
       </c>
       <c r="H146" s="4">
-        <f>H141-30</f>
+        <f t="shared" si="5"/>
         <v>-870</v>
       </c>
       <c r="I146" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K146" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-145 { background: 0px -870px; }</v>
       </c>
     </row>
@@ -10327,14 +10477,14 @@
         <v>0</v>
       </c>
       <c r="H147" s="4">
-        <f>H142-30</f>
+        <f t="shared" si="5"/>
         <v>-870</v>
       </c>
       <c r="I147" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K147" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-146 { background: -0047px -870px; }</v>
       </c>
     </row>
@@ -10361,14 +10511,14 @@
         <v>0</v>
       </c>
       <c r="H148" s="4">
-        <f>H143-30</f>
+        <f t="shared" ref="H148:H179" si="7">H143-30</f>
         <v>-870</v>
       </c>
       <c r="I148" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K148" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-147 { background: -0094px -870px; }</v>
       </c>
     </row>
@@ -10395,14 +10545,14 @@
         <v>0</v>
       </c>
       <c r="H149" s="4">
-        <f>H144-30</f>
+        <f t="shared" si="7"/>
         <v>-870</v>
       </c>
       <c r="I149" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K149" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-148 { background: -0141px -870px; }</v>
       </c>
     </row>
@@ -10429,14 +10579,14 @@
         <v>0</v>
       </c>
       <c r="H150" s="4">
-        <f>H145-30</f>
+        <f t="shared" si="7"/>
         <v>-870</v>
       </c>
       <c r="I150" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K150" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-149 { background: -0188px -870px; }</v>
       </c>
     </row>
@@ -10463,14 +10613,14 @@
         <v>0</v>
       </c>
       <c r="H151" s="4">
-        <f>H146-30</f>
+        <f t="shared" si="7"/>
         <v>-900</v>
       </c>
       <c r="I151" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K151" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-150 { background: 0px -900px; }</v>
       </c>
     </row>
@@ -10497,14 +10647,14 @@
         <v>0</v>
       </c>
       <c r="H152" s="4">
-        <f>H147-30</f>
+        <f t="shared" si="7"/>
         <v>-900</v>
       </c>
       <c r="I152" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K152" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-151 { background: -0047px -900px; }</v>
       </c>
     </row>
@@ -10531,14 +10681,14 @@
         <v>0</v>
       </c>
       <c r="H153" s="4">
-        <f>H148-30</f>
+        <f t="shared" si="7"/>
         <v>-900</v>
       </c>
       <c r="I153" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K153" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-152 { background: -0094px -900px; }</v>
       </c>
     </row>
@@ -10565,14 +10715,14 @@
         <v>0</v>
       </c>
       <c r="H154" s="4">
-        <f>H149-30</f>
+        <f t="shared" si="7"/>
         <v>-900</v>
       </c>
       <c r="I154" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K154" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-153 { background: -0141px -900px; }</v>
       </c>
     </row>
@@ -10599,14 +10749,14 @@
         <v>0</v>
       </c>
       <c r="H155" s="4">
-        <f>H150-30</f>
+        <f t="shared" si="7"/>
         <v>-900</v>
       </c>
       <c r="I155" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K155" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-154 { background: -0188px -900px; }</v>
       </c>
     </row>
@@ -10633,14 +10783,14 @@
         <v>0</v>
       </c>
       <c r="H156" s="4">
-        <f>H151-30</f>
+        <f t="shared" si="7"/>
         <v>-930</v>
       </c>
       <c r="I156" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K156" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-155 { background: 0px -930px; }</v>
       </c>
     </row>
@@ -10667,14 +10817,14 @@
         <v>0</v>
       </c>
       <c r="H157" s="4">
-        <f>H152-30</f>
+        <f t="shared" si="7"/>
         <v>-930</v>
       </c>
       <c r="I157" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K157" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-156 { background: -0047px -930px; }</v>
       </c>
     </row>
@@ -10701,14 +10851,14 @@
         <v>0</v>
       </c>
       <c r="H158" s="4">
-        <f>H153-30</f>
+        <f t="shared" si="7"/>
         <v>-930</v>
       </c>
       <c r="I158" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K158" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-157 { background: -0094px -930px; }</v>
       </c>
     </row>
@@ -10735,14 +10885,14 @@
         <v>0</v>
       </c>
       <c r="H159" s="4">
-        <f>H154-30</f>
+        <f t="shared" si="7"/>
         <v>-930</v>
       </c>
       <c r="I159" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K159" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-158 { background: -0141px -930px; }</v>
       </c>
     </row>
@@ -10769,14 +10919,14 @@
         <v>0</v>
       </c>
       <c r="H160" s="4">
-        <f>H155-30</f>
+        <f t="shared" si="7"/>
         <v>-930</v>
       </c>
       <c r="I160" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K160" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-159 { background: -0188px -930px; }</v>
       </c>
     </row>
@@ -10803,14 +10953,14 @@
         <v>0</v>
       </c>
       <c r="H161" s="4">
-        <f>H156-30</f>
+        <f t="shared" si="7"/>
         <v>-960</v>
       </c>
       <c r="I161" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K161" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-160 { background: 0px -960px; }</v>
       </c>
     </row>
@@ -10837,14 +10987,14 @@
         <v>0</v>
       </c>
       <c r="H162" s="4">
-        <f>H157-30</f>
+        <f t="shared" si="7"/>
         <v>-960</v>
       </c>
       <c r="I162" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K162" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-161 { background: -0047px -960px; }</v>
       </c>
     </row>
@@ -10871,14 +11021,14 @@
         <v>0</v>
       </c>
       <c r="H163" s="4">
-        <f>H158-30</f>
+        <f t="shared" si="7"/>
         <v>-960</v>
       </c>
       <c r="I163" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K163" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-162 { background: -0094px -960px; }</v>
       </c>
     </row>
@@ -10905,14 +11055,14 @@
         <v>0</v>
       </c>
       <c r="H164" s="4">
-        <f>H159-30</f>
+        <f t="shared" si="7"/>
         <v>-960</v>
       </c>
       <c r="I164" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K164" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-163 { background: -0141px -960px; }</v>
       </c>
     </row>
@@ -10939,14 +11089,14 @@
         <v>0</v>
       </c>
       <c r="H165" s="4">
-        <f>H160-30</f>
+        <f t="shared" si="7"/>
         <v>-960</v>
       </c>
       <c r="I165" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K165" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-164 { background: -0188px -960px; }</v>
       </c>
     </row>
@@ -10973,14 +11123,14 @@
         <v>0</v>
       </c>
       <c r="H166" s="4">
-        <f>H161-30</f>
+        <f t="shared" si="7"/>
         <v>-990</v>
       </c>
       <c r="I166" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K166" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-165 { background: 0px -990px; }</v>
       </c>
     </row>
@@ -11007,14 +11157,14 @@
         <v>0</v>
       </c>
       <c r="H167" s="4">
-        <f>H162-30</f>
+        <f t="shared" si="7"/>
         <v>-990</v>
       </c>
       <c r="I167" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K167" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-166 { background: -0047px -990px; }</v>
       </c>
     </row>
@@ -11041,14 +11191,14 @@
         <v>0</v>
       </c>
       <c r="H168" s="4">
-        <f>H163-30</f>
+        <f t="shared" si="7"/>
         <v>-990</v>
       </c>
       <c r="I168" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K168" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-167 { background: -0094px -990px; }</v>
       </c>
     </row>
@@ -11075,14 +11225,14 @@
         <v>0</v>
       </c>
       <c r="H169" s="4">
-        <f>H164-30</f>
+        <f t="shared" si="7"/>
         <v>-990</v>
       </c>
       <c r="I169" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K169" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-168 { background: -0141px -990px; }</v>
       </c>
     </row>
@@ -11109,14 +11259,14 @@
         <v>0</v>
       </c>
       <c r="H170" s="4">
-        <f>H165-30</f>
+        <f t="shared" si="7"/>
         <v>-990</v>
       </c>
       <c r="I170" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K170" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-169 { background: -0188px -990px; }</v>
       </c>
     </row>
@@ -11143,14 +11293,14 @@
         <v>0</v>
       </c>
       <c r="H171" s="4">
-        <f>H166-30</f>
+        <f t="shared" si="7"/>
         <v>-1020</v>
       </c>
       <c r="I171" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K171" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-170 { background: 0px -1020px; }</v>
       </c>
     </row>
@@ -11177,14 +11327,14 @@
         <v>0</v>
       </c>
       <c r="H172" s="4">
-        <f>H167-30</f>
+        <f t="shared" si="7"/>
         <v>-1020</v>
       </c>
       <c r="I172" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K172" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-171 { background: -0047px -1020px; }</v>
       </c>
     </row>
@@ -11211,14 +11361,14 @@
         <v>0</v>
       </c>
       <c r="H173" s="4">
-        <f>H168-30</f>
+        <f t="shared" si="7"/>
         <v>-1020</v>
       </c>
       <c r="I173" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K173" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-172 { background: -0094px -1020px; }</v>
       </c>
     </row>
@@ -11245,14 +11395,14 @@
         <v>0</v>
       </c>
       <c r="H174" s="4">
-        <f>H169-30</f>
+        <f t="shared" si="7"/>
         <v>-1020</v>
       </c>
       <c r="I174" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K174" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-173 { background: -0141px -1020px; }</v>
       </c>
     </row>
@@ -11279,14 +11429,14 @@
         <v>0</v>
       </c>
       <c r="H175" s="4">
-        <f>H170-30</f>
+        <f t="shared" si="7"/>
         <v>-1020</v>
       </c>
       <c r="I175" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K175" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-174 { background: -0188px -1020px; }</v>
       </c>
     </row>
@@ -11313,14 +11463,14 @@
         <v>0</v>
       </c>
       <c r="H176" s="4">
-        <f>H171-30</f>
+        <f t="shared" si="7"/>
         <v>-1050</v>
       </c>
       <c r="I176" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K176" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-175 { background: 0px -1050px; }</v>
       </c>
     </row>
@@ -11347,14 +11497,14 @@
         <v>0</v>
       </c>
       <c r="H177" s="4">
-        <f>H172-30</f>
+        <f t="shared" si="7"/>
         <v>-1050</v>
       </c>
       <c r="I177" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K177" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-176 { background: -0047px -1050px; }</v>
       </c>
     </row>
@@ -11381,14 +11531,14 @@
         <v>0</v>
       </c>
       <c r="H178" s="4">
-        <f>H173-30</f>
+        <f t="shared" si="7"/>
         <v>-1050</v>
       </c>
       <c r="I178" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K178" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-177 { background: -0094px -1050px; }</v>
       </c>
     </row>
@@ -11415,14 +11565,14 @@
         <v>0</v>
       </c>
       <c r="H179" s="4">
-        <f>H174-30</f>
+        <f t="shared" si="7"/>
         <v>-1050</v>
       </c>
       <c r="I179" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K179" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-178 { background: -0141px -1050px; }</v>
       </c>
     </row>
@@ -11449,14 +11599,14 @@
         <v>0</v>
       </c>
       <c r="H180" s="4">
-        <f>H175-30</f>
+        <f t="shared" ref="H180:H211" si="8">H175-30</f>
         <v>-1050</v>
       </c>
       <c r="I180" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K180" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-179 { background: -0188px -1050px; }</v>
       </c>
     </row>
@@ -11483,14 +11633,14 @@
         <v>0</v>
       </c>
       <c r="H181" s="4">
-        <f>H176-30</f>
+        <f t="shared" si="8"/>
         <v>-1080</v>
       </c>
       <c r="I181" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K181" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-180 { background: 0px -1080px; }</v>
       </c>
     </row>
@@ -11517,14 +11667,14 @@
         <v>0</v>
       </c>
       <c r="H182" s="4">
-        <f>H177-30</f>
+        <f t="shared" si="8"/>
         <v>-1080</v>
       </c>
       <c r="I182" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K182" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-181 { background: -0047px -1080px; }</v>
       </c>
     </row>
@@ -11551,14 +11701,14 @@
         <v>0</v>
       </c>
       <c r="H183" s="4">
-        <f>H178-30</f>
+        <f t="shared" si="8"/>
         <v>-1080</v>
       </c>
       <c r="I183" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K183" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-182 { background: -0094px -1080px; }</v>
       </c>
     </row>
@@ -11585,14 +11735,14 @@
         <v>0</v>
       </c>
       <c r="H184" s="4">
-        <f>H179-30</f>
+        <f t="shared" si="8"/>
         <v>-1080</v>
       </c>
       <c r="I184" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K184" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-183 { background: -0141px -1080px; }</v>
       </c>
     </row>
@@ -11619,14 +11769,14 @@
         <v>0</v>
       </c>
       <c r="H185" s="4">
-        <f>H180-30</f>
+        <f t="shared" si="8"/>
         <v>-1080</v>
       </c>
       <c r="I185" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K185" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-184 { background: -0188px -1080px; }</v>
       </c>
     </row>
@@ -11653,14 +11803,14 @@
         <v>0</v>
       </c>
       <c r="H186" s="4">
-        <f>H181-30</f>
+        <f t="shared" si="8"/>
         <v>-1110</v>
       </c>
       <c r="I186" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K186" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-185 { background: 0px -1110px; }</v>
       </c>
     </row>
@@ -11687,14 +11837,14 @@
         <v>0</v>
       </c>
       <c r="H187" s="4">
-        <f>H182-30</f>
+        <f t="shared" si="8"/>
         <v>-1110</v>
       </c>
       <c r="I187" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K187" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-186 { background: -0047px -1110px; }</v>
       </c>
     </row>
@@ -11721,14 +11871,14 @@
         <v>0</v>
       </c>
       <c r="H188" s="4">
-        <f>H183-30</f>
+        <f t="shared" si="8"/>
         <v>-1110</v>
       </c>
       <c r="I188" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K188" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-187 { background: -0094px -1110px; }</v>
       </c>
     </row>
@@ -11755,14 +11905,14 @@
         <v>0</v>
       </c>
       <c r="H189" s="4">
-        <f>H184-30</f>
+        <f t="shared" si="8"/>
         <v>-1110</v>
       </c>
       <c r="I189" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K189" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-188 { background: -0141px -1110px; }</v>
       </c>
     </row>
@@ -11789,14 +11939,14 @@
         <v>0</v>
       </c>
       <c r="H190" s="4">
-        <f>H185-30</f>
+        <f t="shared" si="8"/>
         <v>-1110</v>
       </c>
       <c r="I190" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K190" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-189 { background: -0188px -1110px; }</v>
       </c>
     </row>
@@ -11823,14 +11973,14 @@
         <v>0</v>
       </c>
       <c r="H191" s="4">
-        <f>H186-30</f>
+        <f t="shared" si="8"/>
         <v>-1140</v>
       </c>
       <c r="I191" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K191" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-190 { background: 0px -1140px; }</v>
       </c>
     </row>
@@ -11857,14 +12007,14 @@
         <v>0</v>
       </c>
       <c r="H192" s="4">
-        <f>H187-30</f>
+        <f t="shared" si="8"/>
         <v>-1140</v>
       </c>
       <c r="I192" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K192" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-191 { background: -0047px -1140px; }</v>
       </c>
     </row>
@@ -11891,14 +12041,14 @@
         <v>0</v>
       </c>
       <c r="H193" s="4">
-        <f>H188-30</f>
+        <f t="shared" si="8"/>
         <v>-1140</v>
       </c>
       <c r="I193" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K193" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>.flair-192 { background: -0094px -1140px; }</v>
       </c>
     </row>
@@ -11925,14 +12075,14 @@
         <v>0</v>
       </c>
       <c r="H194" s="4">
-        <f>H189-30</f>
+        <f t="shared" si="8"/>
         <v>-1140</v>
       </c>
       <c r="I194" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K194" s="1" t="str">
-        <f t="shared" ref="K194:K200" si="3">A194&amp;B194&amp;C194&amp;D194&amp;E194&amp;F194&amp;G194&amp;H194&amp;I194</f>
+        <f t="shared" ref="K194:K200" si="9">A194&amp;B194&amp;C194&amp;D194&amp;E194&amp;F194&amp;G194&amp;H194&amp;I194</f>
         <v>.flair-193 { background: -0141px -1140px; }</v>
       </c>
     </row>
@@ -11959,14 +12109,14 @@
         <v>0</v>
       </c>
       <c r="H195" s="4">
-        <f>H190-30</f>
+        <f t="shared" si="8"/>
         <v>-1140</v>
       </c>
       <c r="I195" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K195" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>.flair-194 { background: -0188px -1140px; }</v>
       </c>
     </row>
@@ -11993,14 +12143,14 @@
         <v>0</v>
       </c>
       <c r="H196" s="4">
-        <f>H191-30</f>
+        <f t="shared" si="8"/>
         <v>-1170</v>
       </c>
       <c r="I196" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K196" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>.flair-195 { background: 0px -1170px; }</v>
       </c>
     </row>
@@ -12027,14 +12177,14 @@
         <v>0</v>
       </c>
       <c r="H197" s="4">
-        <f>H192-30</f>
+        <f t="shared" si="8"/>
         <v>-1170</v>
       </c>
       <c r="I197" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K197" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>.flair-196 { background: -0047px -1170px; }</v>
       </c>
     </row>
@@ -12061,14 +12211,14 @@
         <v>0</v>
       </c>
       <c r="H198" s="4">
-        <f>H193-30</f>
+        <f t="shared" si="8"/>
         <v>-1170</v>
       </c>
       <c r="I198" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K198" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>.flair-197 { background: -0094px -1170px; }</v>
       </c>
     </row>
@@ -12095,14 +12245,14 @@
         <v>0</v>
       </c>
       <c r="H199" s="4">
-        <f>H194-30</f>
+        <f t="shared" si="8"/>
         <v>-1170</v>
       </c>
       <c r="I199" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K199" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>.flair-198 { background: -0141px -1170px; }</v>
       </c>
     </row>
@@ -12129,14 +12279,14 @@
         <v>0</v>
       </c>
       <c r="H200" s="4">
-        <f>H195-30</f>
+        <f t="shared" si="8"/>
         <v>-1170</v>
       </c>
       <c r="I200" s="1" t="s">
         <v>4</v>
       </c>
       <c r="K200" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>.flair-199 { background: -0188px -1170px; }</v>
       </c>
     </row>

</xml_diff>